<commit_message>
finally have a topic and analysis just need approval
</commit_message>
<xml_diff>
--- a/data/data dictionary.xlsx
+++ b/data/data dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunhe\Documents\NSS\final_capstone_public_transportation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AF9A49-B9CA-4DA6-B28E-56070C478FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502F566C-9861-4151-852E-27212E1FB1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="568" xr2:uid="{4010D8FD-1B1E-4FE8-B00A-2CABB5026443}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
   <si>
     <t>Term</t>
   </si>
@@ -335,6 +335,83 @@
   </si>
   <si>
     <t>ID number given by state.  It looks like it does not match the state column that I added.</t>
+  </si>
+  <si>
+    <t>VRM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vehicle Revenue Miles The miles that vehicles are scheduled to or actually travel while in revenue service. Vehicle revenue miles </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>include</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Layover / recovery time.
+Vehicle revenue miles </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exclude</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Deadhead, Operator training, Vehicle maintenance testing, and Other non-revenue uses of vehicles.</t>
+    </r>
+  </si>
+  <si>
+    <t>Vehicle Revenue Hours (VRH)
+The hours that vehicles are scheduled to or actually travel while in revenue service. Vehicle revenue hours include: 
+•   Layover / recovery time.
+Vehicle revenue hours exclude: 
+•   Deadhead;
+•   Operator training;
+•   Vehicle maintenance testing; and
+•   Other non-revenue uses of vehicles.</t>
+  </si>
+  <si>
+    <t>VRH</t>
+  </si>
+  <si>
+    <t>Unlinked Passenger Trips (UPT)
+The number of passengers who board public transportation vehicles. Passengers are counted each time they board vehicles no matter how many vehicles they use to travel from their origin to their destination. Can be found in: F-10, S-10, FFA-10, Declarations, MR-20</t>
+  </si>
+  <si>
+    <t>Unlinked Passenger Trips (UPT)</t>
+  </si>
+  <si>
+    <t>PMT</t>
+  </si>
+  <si>
+    <t>Passenger Miles Traveled</t>
   </si>
 </sst>
 </file>
@@ -425,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -458,9 +535,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10753A4A-94A6-4B74-85AA-564FBB93BF7C}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -879,42 +959,44 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="8" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="189.45" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -927,122 +1009,122 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="8" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A22" s="8" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A23" s="8" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="8" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" s="8" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A30" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="4" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -1053,129 +1135,162 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A36" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A38" s="8" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A39" s="8" t="s">
+    <row r="41" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A41" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A40" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A41" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A42" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A43" s="8" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A45" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A47" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A48" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B49" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A45" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A46" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>93</v>
-      </c>
+    <row r="50" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A50" s="8"/>
+      <c r="B50" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{10753A4A-94A6-4B74-85AA-564FBB93BF7C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B50">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -1206,10 +1321,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>